<commit_message>
Update excel til 14 dage
</commit_message>
<xml_diff>
--- a/Regneark/produktion.xlsx
+++ b/Regneark/produktion.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrj/Nextcloud/Undervisning/Kerteminde/kolding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrj/Git/EnergiCase/Regneark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D757D5A-D042-DD4B-980A-D710DE63691C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D24A52-8AFE-0941-9E5F-4B6D03495119}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="4680" windowWidth="17220" windowHeight="12540" xr2:uid="{78A2D073-3E73-0045-A426-782D5B90BEAC}"/>
+    <workbookView xWindow="-25540" yWindow="-9120" windowWidth="20680" windowHeight="17540" xr2:uid="{78A2D073-3E73-0045-A426-782D5B90BEAC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="data">Sheet1!$C$2:$F$313</definedName>
+    <definedName name="data">Sheet1!$C$2:$F$337</definedName>
     <definedName name="kolone">Sheet1!$C$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -480,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9C7061-77DC-D14E-AAC3-0E8041FA3D9D}">
-  <dimension ref="A1:F313"/>
+  <dimension ref="A1:F337"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
+      <selection activeCell="I334" sqref="I334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6748,6 +6748,486 @@
         <v>2169.1</v>
       </c>
     </row>
+    <row r="314" spans="1:6">
+      <c r="A314" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B314" s="4">
+        <v>1</v>
+      </c>
+      <c r="C314" s="5">
+        <v>468.7</v>
+      </c>
+      <c r="D314" s="5">
+        <v>1393</v>
+      </c>
+      <c r="E314" s="5">
+        <v>0</v>
+      </c>
+      <c r="F314" s="5">
+        <v>2076.9</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6">
+      <c r="A315" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B315" s="4">
+        <v>2</v>
+      </c>
+      <c r="C315" s="5">
+        <v>451.6</v>
+      </c>
+      <c r="D315" s="5">
+        <v>1375.9</v>
+      </c>
+      <c r="E315" s="5">
+        <v>0</v>
+      </c>
+      <c r="F315" s="5">
+        <v>2018.6</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6">
+      <c r="A316" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B316" s="4">
+        <v>3</v>
+      </c>
+      <c r="C316" s="5">
+        <v>451.2</v>
+      </c>
+      <c r="D316" s="5">
+        <v>1433.5</v>
+      </c>
+      <c r="E316" s="5">
+        <v>0</v>
+      </c>
+      <c r="F316" s="5">
+        <v>1984.1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6">
+      <c r="A317" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B317" s="4">
+        <v>4</v>
+      </c>
+      <c r="C317" s="5">
+        <v>432.5</v>
+      </c>
+      <c r="D317" s="5">
+        <v>1511.3</v>
+      </c>
+      <c r="E317" s="5">
+        <v>0</v>
+      </c>
+      <c r="F317" s="5">
+        <v>1969.6</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6">
+      <c r="A318" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B318" s="4">
+        <v>5</v>
+      </c>
+      <c r="C318" s="5">
+        <v>427.8</v>
+      </c>
+      <c r="D318" s="5">
+        <v>1625.5</v>
+      </c>
+      <c r="E318" s="5">
+        <v>0</v>
+      </c>
+      <c r="F318" s="5">
+        <v>1994.7</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6">
+      <c r="A319" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B319" s="4">
+        <v>6</v>
+      </c>
+      <c r="C319" s="5">
+        <v>446</v>
+      </c>
+      <c r="D319" s="5">
+        <v>1646.7</v>
+      </c>
+      <c r="E319" s="5">
+        <v>0</v>
+      </c>
+      <c r="F319" s="5">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6">
+      <c r="A320" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B320" s="4">
+        <v>7</v>
+      </c>
+      <c r="C320" s="5">
+        <v>510.8</v>
+      </c>
+      <c r="D320" s="5">
+        <v>1479.8</v>
+      </c>
+      <c r="E320" s="5">
+        <v>0</v>
+      </c>
+      <c r="F320" s="5">
+        <v>2170.6999999999998</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6">
+      <c r="A321" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B321" s="4">
+        <v>8</v>
+      </c>
+      <c r="C321" s="5">
+        <v>539.9</v>
+      </c>
+      <c r="D321" s="5">
+        <v>1597.9</v>
+      </c>
+      <c r="E321" s="5">
+        <v>0</v>
+      </c>
+      <c r="F321" s="5">
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6">
+      <c r="A322" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B322" s="4">
+        <v>9</v>
+      </c>
+      <c r="C322" s="5">
+        <v>567.1</v>
+      </c>
+      <c r="D322" s="5">
+        <v>1671.4</v>
+      </c>
+      <c r="E322" s="5">
+        <v>0</v>
+      </c>
+      <c r="F322" s="5">
+        <v>2541.9</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6">
+      <c r="A323" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B323" s="4">
+        <v>10</v>
+      </c>
+      <c r="C323" s="5">
+        <v>580.5</v>
+      </c>
+      <c r="D323" s="5">
+        <v>1596.8</v>
+      </c>
+      <c r="E323" s="5">
+        <v>2</v>
+      </c>
+      <c r="F323" s="5">
+        <v>2626.3</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6">
+      <c r="A324" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B324" s="4">
+        <v>11</v>
+      </c>
+      <c r="C324" s="5">
+        <v>599.6</v>
+      </c>
+      <c r="D324" s="5">
+        <v>1412.5</v>
+      </c>
+      <c r="E324" s="5">
+        <v>11</v>
+      </c>
+      <c r="F324" s="5">
+        <v>2682</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6">
+      <c r="A325" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B325" s="4">
+        <v>12</v>
+      </c>
+      <c r="C325" s="5">
+        <v>607.1</v>
+      </c>
+      <c r="D325" s="5">
+        <v>1283.2</v>
+      </c>
+      <c r="E325" s="5">
+        <v>19</v>
+      </c>
+      <c r="F325" s="5">
+        <v>2679.7</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6">
+      <c r="A326" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B326" s="4">
+        <v>13</v>
+      </c>
+      <c r="C326" s="5">
+        <v>606.29999999999995</v>
+      </c>
+      <c r="D326" s="5">
+        <v>1254.2</v>
+      </c>
+      <c r="E326" s="5">
+        <v>24</v>
+      </c>
+      <c r="F326" s="5">
+        <v>2628.4</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6">
+      <c r="A327" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B327" s="4">
+        <v>14</v>
+      </c>
+      <c r="C327" s="5">
+        <v>592</v>
+      </c>
+      <c r="D327" s="5">
+        <v>1342.8</v>
+      </c>
+      <c r="E327" s="5">
+        <v>23</v>
+      </c>
+      <c r="F327" s="5">
+        <v>2580.9</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6">
+      <c r="A328" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B328" s="4">
+        <v>15</v>
+      </c>
+      <c r="C328" s="5">
+        <v>576.20000000000005</v>
+      </c>
+      <c r="D328" s="5">
+        <v>1487.5</v>
+      </c>
+      <c r="E328" s="5">
+        <v>13</v>
+      </c>
+      <c r="F328" s="5">
+        <v>2561.1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6">
+      <c r="A329" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B329" s="4">
+        <v>16</v>
+      </c>
+      <c r="C329" s="5">
+        <v>570.5</v>
+      </c>
+      <c r="D329" s="5">
+        <v>1776.7</v>
+      </c>
+      <c r="E329" s="5">
+        <v>2</v>
+      </c>
+      <c r="F329" s="5">
+        <v>2606.6</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6">
+      <c r="A330" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B330" s="4">
+        <v>17</v>
+      </c>
+      <c r="C330" s="5">
+        <v>576.79999999999995</v>
+      </c>
+      <c r="D330" s="5">
+        <v>1843.6</v>
+      </c>
+      <c r="E330" s="5">
+        <v>0</v>
+      </c>
+      <c r="F330" s="5">
+        <v>2746.5</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6">
+      <c r="A331" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B331" s="4">
+        <v>18</v>
+      </c>
+      <c r="C331" s="5">
+        <v>563.70000000000005</v>
+      </c>
+      <c r="D331" s="5">
+        <v>2032.7</v>
+      </c>
+      <c r="E331" s="5">
+        <v>0</v>
+      </c>
+      <c r="F331" s="5">
+        <v>2882.7</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6">
+      <c r="A332" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B332" s="4">
+        <v>19</v>
+      </c>
+      <c r="C332" s="5">
+        <v>567.4</v>
+      </c>
+      <c r="D332" s="5">
+        <v>2324.8000000000002</v>
+      </c>
+      <c r="E332" s="5">
+        <v>0</v>
+      </c>
+      <c r="F332" s="5">
+        <v>2804.2</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6">
+      <c r="A333" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B333" s="4">
+        <v>20</v>
+      </c>
+      <c r="C333" s="5">
+        <v>539.70000000000005</v>
+      </c>
+      <c r="D333" s="5">
+        <v>2509.4</v>
+      </c>
+      <c r="E333" s="5">
+        <v>0</v>
+      </c>
+      <c r="F333" s="5">
+        <v>2631</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6">
+      <c r="A334" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B334" s="4">
+        <v>21</v>
+      </c>
+      <c r="C334" s="5">
+        <v>445.3</v>
+      </c>
+      <c r="D334" s="5">
+        <v>2677.9</v>
+      </c>
+      <c r="E334" s="5">
+        <v>0</v>
+      </c>
+      <c r="F334" s="5">
+        <v>2498.9</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6">
+      <c r="A335" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B335" s="4">
+        <v>22</v>
+      </c>
+      <c r="C335" s="5">
+        <v>321.8</v>
+      </c>
+      <c r="D335" s="5">
+        <v>3023.8</v>
+      </c>
+      <c r="E335" s="5">
+        <v>0</v>
+      </c>
+      <c r="F335" s="5">
+        <v>2382.6</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6">
+      <c r="A336" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B336" s="4">
+        <v>23</v>
+      </c>
+      <c r="C336" s="5">
+        <v>293.60000000000002</v>
+      </c>
+      <c r="D336" s="5">
+        <v>3221.4</v>
+      </c>
+      <c r="E336" s="5">
+        <v>0</v>
+      </c>
+      <c r="F336" s="5">
+        <v>2273.3000000000002</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6">
+      <c r="A337" s="3">
+        <v>43813</v>
+      </c>
+      <c r="B337" s="4">
+        <v>24</v>
+      </c>
+      <c r="C337" s="5">
+        <v>256.2</v>
+      </c>
+      <c r="D337" s="5">
+        <v>3345.9</v>
+      </c>
+      <c r="E337" s="5">
+        <v>0</v>
+      </c>
+      <c r="F337" s="5">
+        <v>2297.1999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>